<commit_message>
Use zip to create multiple files
</commit_message>
<xml_diff>
--- a/templates/export/individual_device_report.xlsx
+++ b/templates/export/individual_device_report.xlsx
@@ -44,20 +44,6 @@
           </rPr>
           <t xml:space="preserve">jx:area(lastCell="D90")
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="D90")</t>
         </r>
       </text>
     </comment>
@@ -535,6 +521,21 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -553,23 +554,8 @@
     <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -859,7 +845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A50" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A55" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="120" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -874,23 +860,23 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:7" ht="46" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="24"/>
+      <c r="D3" s="29"/>
       <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.25">
@@ -904,18 +890,18 @@
       <c r="B6" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
     </row>
     <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
     </row>
     <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
@@ -943,37 +929,37 @@
       <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
       <c r="G15" s="13"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
@@ -1024,20 +1010,20 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.2">
-      <c r="A45" s="30" t="s">
+      <c r="A45" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
     </row>
     <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A46" s="31" t="s">
+      <c r="A46" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
     </row>
     <row r="47" spans="1:4" ht="37" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2"/>
@@ -1054,10 +1040,10 @@
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="27">
+      <c r="A49" s="21">
         <v>1</v>
       </c>
-      <c r="B49" s="32" t="s">
+      <c r="B49" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C49" s="19" t="s">
@@ -1068,8 +1054,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="27"/>
-      <c r="B50" s="32"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="25"/>
       <c r="C50" s="19" t="s">
         <v>2</v>
       </c>
@@ -1078,10 +1064,10 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="27">
+      <c r="A51" s="21">
         <v>2</v>
       </c>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="22" t="s">
         <v>38</v>
       </c>
       <c r="C51" s="19" t="s">
@@ -1092,8 +1078,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="27"/>
-      <c r="B52" s="28"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="22"/>
       <c r="C52" s="20" t="s">
         <v>33</v>
       </c>
@@ -1102,8 +1088,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="27"/>
-      <c r="B53" s="28"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="22"/>
       <c r="C53" s="19" t="s">
         <v>28</v>
       </c>
@@ -1112,8 +1098,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="27"/>
-      <c r="B54" s="28"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="22"/>
       <c r="C54" s="19" t="s">
         <v>4</v>
       </c>
@@ -1122,8 +1108,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="27"/>
-      <c r="B55" s="28"/>
+      <c r="A55" s="21"/>
+      <c r="B55" s="22"/>
       <c r="C55" s="19" t="s">
         <v>20</v>
       </c>
@@ -1132,8 +1118,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="27"/>
-      <c r="B56" s="28"/>
+      <c r="A56" s="21"/>
+      <c r="B56" s="22"/>
       <c r="C56" s="19" t="s">
         <v>21</v>
       </c>
@@ -1142,8 +1128,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="27"/>
-      <c r="B57" s="28"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="22"/>
       <c r="C57" s="19" t="s">
         <v>24</v>
       </c>
@@ -1152,10 +1138,10 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="27">
+      <c r="A58" s="21">
         <v>3</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="22" t="s">
         <v>22</v>
       </c>
       <c r="C58" s="19" t="s">
@@ -1166,8 +1152,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="27"/>
-      <c r="B59" s="28"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="22"/>
       <c r="C59" s="19" t="s">
         <v>30</v>
       </c>
@@ -1176,8 +1162,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="27"/>
-      <c r="B60" s="28"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="22"/>
       <c r="C60" s="19" t="s">
         <v>31</v>
       </c>
@@ -1186,8 +1172,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="27"/>
-      <c r="B61" s="28"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="22"/>
       <c r="C61" s="19" t="s">
         <v>34</v>
       </c>
@@ -1196,8 +1182,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="27"/>
-      <c r="B62" s="28"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="22"/>
       <c r="C62" s="19" t="s">
         <v>32</v>
       </c>
@@ -1206,8 +1192,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="27"/>
-      <c r="B63" s="28"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="22"/>
       <c r="C63" s="19" t="s">
         <v>25</v>
       </c>
@@ -1217,12 +1203,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A58:A63"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A46:D46"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
     <mergeCell ref="A15:D19"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
@@ -1231,6 +1211,12 @@
     <mergeCell ref="B51:B57"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A58:A63"/>
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A46:D46"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>